<commit_message>
branding changes of wave tool recommended
</commit_message>
<xml_diff>
--- a/clients/html/src/assets/roster_upload_template_me.xlsx
+++ b/clients/html/src/assets/roster_upload_template_me.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11113"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34DE079-ED4E-F847-897D-1C005CF57FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C542034-C05D-034C-9C00-32197FD67C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="25600" windowHeight="14540" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -511,13 +511,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF005E81"/>
+        <fgColor rgb="FF6D6E70"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6D6E70"/>
+        <fgColor rgb="FF3C5E6E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,37 +808,37 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="18" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="28" fillId="18" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="78"/>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="19" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="28" fillId="19" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="78"/>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="32" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="20% - Accent1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -936,6 +936,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3C5E6E"/>
       <color rgb="FF005E81"/>
       <color rgb="FF6D6E70"/>
       <color rgb="FFDDEEFF"/>
@@ -1245,7 +1246,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1271,23 +1272,23 @@
     <col min="22" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="21" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:21" s="24" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="27">
+      <c r="H1" s="25">
         <v>42669</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="N1" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="23"/>
+      <c r="U1" s="28"/>
     </row>
     <row r="2" spans="1:21" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1350,41 +1351,41 @@
       <c r="T2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="19" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:21" s="18" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="25"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="21"/>
     </row>
     <row r="4" spans="1:21" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1393,7 +1394,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="5"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>

</xml_diff>

<commit_message>
branding for aeqt (#50)
* branding for aeqt

* branding changes of wave tool recommended
</commit_message>
<xml_diff>
--- a/clients/html/src/assets/roster_upload_template_me.xlsx
+++ b/clients/html/src/assets/roster_upload_template_me.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11113"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34DE079-ED4E-F847-897D-1C005CF57FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C542034-C05D-034C-9C00-32197FD67C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="25600" windowHeight="14540" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -511,13 +511,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF005E81"/>
+        <fgColor rgb="FF6D6E70"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6D6E70"/>
+        <fgColor rgb="FF3C5E6E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,37 +808,37 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="18" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="28" fillId="18" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="78"/>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="19" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="28" fillId="19" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="31" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="78"/>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="32" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="31" fillId="19" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="20% - Accent1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -936,6 +936,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3C5E6E"/>
       <color rgb="FF005E81"/>
       <color rgb="FF6D6E70"/>
       <color rgb="FFDDEEFF"/>
@@ -1245,7 +1246,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1271,23 +1272,23 @@
     <col min="22" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="21" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:21" s="24" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="27">
+      <c r="H1" s="25">
         <v>42669</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="N1" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="23"/>
+      <c r="U1" s="28"/>
     </row>
     <row r="2" spans="1:21" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1350,41 +1351,41 @@
       <c r="T2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="19" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:21" s="18" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="25"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="21"/>
     </row>
     <row r="4" spans="1:21" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1393,7 +1394,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="5"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>

</xml_diff>